<commit_message>
Moved the raw profiling to the profiling folder and added some consolidated results in the excel spreadsheet.
</commit_message>
<xml_diff>
--- a/java_implementation/profiling/data_table.xlsx
+++ b/java_implementation/profiling/data_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Pipes</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t>Highest Throughput:</t>
+  </si>
+  <si>
+    <t>Overall Average Throughput:</t>
+  </si>
+  <si>
+    <t>Average Throughput</t>
+  </si>
+  <si>
+    <t>Highest Throughput</t>
   </si>
 </sst>
 </file>
@@ -376,21 +385,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H261"/>
+  <dimension ref="A1:I261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.36328125" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" customWidth="1"/>
+    <col min="9" max="9" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -407,7 +420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -431,7 +444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -447,8 +460,15 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <f>AVERAGE(E2:E261)</f>
+        <v>18.761538461538461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -465,7 +485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -481,8 +501,17 @@
       <c r="E5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -498,8 +527,19 @@
       <c r="E6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(E2:E41)</f>
+        <v>8.375</v>
+      </c>
+      <c r="I6">
+        <f>MAX(E2:E41)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -515,8 +555,19 @@
       <c r="E7" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(E42:E81)</f>
+        <v>11.824999999999999</v>
+      </c>
+      <c r="I7">
+        <f>MAX(E42:E81)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -532,8 +583,19 @@
       <c r="E8" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(E82:E121)</f>
+        <v>16.350000000000001</v>
+      </c>
+      <c r="I8">
+        <f>MAX(E82:E121)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -549,8 +611,19 @@
       <c r="E9" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f>AVERAGE(E122:E161)</f>
+        <v>22</v>
+      </c>
+      <c r="I9">
+        <f>MAX(E122:E161)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -566,8 +639,19 @@
       <c r="E10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f>AVERAGE(E162:E201)</f>
+        <v>16.2</v>
+      </c>
+      <c r="I10">
+        <f>MAX(E162:E201)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -583,8 +667,19 @@
       <c r="E11" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <f>AVERAGE(E202:E231)</f>
+        <v>31.7</v>
+      </c>
+      <c r="I11">
+        <f>MAX(E202:E231)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -600,8 +695,19 @@
       <c r="E12" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <f>AVERAGE(E232:E261)</f>
+        <v>31.233333333333334</v>
+      </c>
+      <c r="I12">
+        <f>MAX(E232:E261)</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -618,7 +724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -635,7 +741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -652,7 +758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -669,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -686,7 +792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -703,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -720,7 +826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -737,7 +843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -754,7 +860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -771,7 +877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -788,7 +894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -805,7 +911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -822,7 +928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -839,7 +945,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -856,7 +962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -873,7 +979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -890,7 +996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -907,7 +1013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -924,7 +1030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -941,7 +1047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -958,7 +1064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -975,7 +1081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -992,7 +1098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1009,7 +1115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -1026,7 +1132,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -1043,7 +1149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -1060,7 +1166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -1077,7 +1183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -1094,7 +1200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -1111,7 +1217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>2</v>
       </c>
@@ -1128,7 +1234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>2</v>
       </c>
@@ -1145,7 +1251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>2</v>
       </c>
@@ -1162,7 +1268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -1179,7 +1285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>2</v>
       </c>
@@ -1196,7 +1302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>2</v>
       </c>
@@ -1213,7 +1319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>2</v>
       </c>
@@ -1230,7 +1336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>2</v>
       </c>
@@ -1247,7 +1353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>2</v>
       </c>
@@ -1264,7 +1370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>2</v>
       </c>
@@ -1281,7 +1387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>2</v>
       </c>
@@ -1298,7 +1404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>2</v>
       </c>
@@ -1315,7 +1421,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>2</v>
       </c>
@@ -1332,7 +1438,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>2</v>
       </c>
@@ -1349,7 +1455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>2</v>
       </c>
@@ -1366,7 +1472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2</v>
       </c>
@@ -1383,7 +1489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>2</v>
       </c>
@@ -1400,7 +1506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>2</v>
       </c>
@@ -1417,7 +1523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>2</v>
       </c>
@@ -1434,7 +1540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>2</v>
       </c>
@@ -1451,7 +1557,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>2</v>
       </c>
@@ -1468,7 +1574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>2</v>
       </c>
@@ -1485,7 +1591,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>2</v>
       </c>
@@ -1502,7 +1608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>2</v>
       </c>
@@ -1519,7 +1625,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>2</v>
       </c>
@@ -1536,7 +1642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>2</v>
       </c>
@@ -1553,7 +1659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>2</v>
       </c>
@@ -1570,7 +1676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>2</v>
       </c>
@@ -1587,7 +1693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>2</v>
       </c>
@@ -1604,7 +1710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>2</v>
       </c>
@@ -1621,7 +1727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>2</v>
       </c>
@@ -1638,7 +1744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>2</v>
       </c>
@@ -1655,7 +1761,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>2</v>
       </c>
@@ -1672,7 +1778,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>2</v>
       </c>
@@ -1689,7 +1795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>2</v>
       </c>
@@ -1706,7 +1812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>2</v>
       </c>
@@ -1723,7 +1829,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>2</v>
       </c>
@@ -1740,7 +1846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>2</v>
       </c>
@@ -1757,7 +1863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>2</v>
       </c>
@@ -1774,7 +1880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>3</v>
       </c>
@@ -1791,7 +1897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>3</v>
       </c>
@@ -1808,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>3</v>
       </c>
@@ -1825,7 +1931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>3</v>
       </c>
@@ -1842,7 +1948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>3</v>
       </c>
@@ -1859,7 +1965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>3</v>
       </c>
@@ -1876,7 +1982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>3</v>
       </c>
@@ -1893,7 +1999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>3</v>
       </c>
@@ -1910,7 +2016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>3</v>
       </c>
@@ -1927,7 +2033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>3</v>
       </c>
@@ -1944,7 +2050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>3</v>
       </c>
@@ -1961,7 +2067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>3</v>
       </c>
@@ -1978,7 +2084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>3</v>
       </c>
@@ -1995,7 +2101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>3</v>
       </c>
@@ -2012,7 +2118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>3</v>
       </c>
@@ -2029,7 +2135,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>3</v>
       </c>
@@ -2046,7 +2152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>3</v>
       </c>
@@ -2063,7 +2169,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>3</v>
       </c>
@@ -2080,7 +2186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>3</v>
       </c>
@@ -2097,7 +2203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>3</v>
       </c>
@@ -2114,7 +2220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>3</v>
       </c>
@@ -2131,7 +2237,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>3</v>
       </c>
@@ -2148,7 +2254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>3</v>
       </c>
@@ -2165,7 +2271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>3</v>
       </c>
@@ -2182,7 +2288,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>3</v>
       </c>
@@ -2199,7 +2305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>3</v>
       </c>
@@ -2216,7 +2322,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>3</v>
       </c>
@@ -2233,7 +2339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>3</v>
       </c>
@@ -2250,7 +2356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>3</v>
       </c>
@@ -2267,7 +2373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>3</v>
       </c>
@@ -2284,7 +2390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>3</v>
       </c>
@@ -2301,7 +2407,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>3</v>
       </c>
@@ -2318,7 +2424,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>3</v>
       </c>
@@ -2335,7 +2441,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>3</v>
       </c>
@@ -2352,7 +2458,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>3</v>
       </c>
@@ -2369,7 +2475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>3</v>
       </c>
@@ -2386,7 +2492,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>3</v>
       </c>
@@ -2403,7 +2509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>3</v>
       </c>
@@ -2420,7 +2526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>3</v>
       </c>
@@ -2437,7 +2543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>3</v>
       </c>
@@ -2454,7 +2560,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>4</v>
       </c>
@@ -2471,7 +2577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>4</v>
       </c>
@@ -2488,7 +2594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>4</v>
       </c>
@@ -2505,7 +2611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>4</v>
       </c>
@@ -2522,7 +2628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>4</v>
       </c>
@@ -2539,7 +2645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>4</v>
       </c>
@@ -2556,7 +2662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>4</v>
       </c>
@@ -2573,7 +2679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>4</v>
       </c>
@@ -2590,7 +2696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>4</v>
       </c>
@@ -2607,7 +2713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>4</v>
       </c>
@@ -2624,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>4</v>
       </c>
@@ -2641,7 +2747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>4</v>
       </c>
@@ -2658,7 +2764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>4</v>
       </c>
@@ -2675,7 +2781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>4</v>
       </c>
@@ -2692,7 +2798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>4</v>
       </c>
@@ -2709,7 +2815,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>4</v>
       </c>
@@ -2726,7 +2832,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>4</v>
       </c>
@@ -2743,7 +2849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>4</v>
       </c>
@@ -2760,7 +2866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>4</v>
       </c>
@@ -2777,7 +2883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>4</v>
       </c>
@@ -2794,7 +2900,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>4</v>
       </c>
@@ -2811,7 +2917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>4</v>
       </c>
@@ -2828,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>4</v>
       </c>
@@ -2845,7 +2951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>4</v>
       </c>
@@ -2862,7 +2968,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>4</v>
       </c>
@@ -2879,7 +2985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>4</v>
       </c>
@@ -2896,7 +3002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>4</v>
       </c>
@@ -2913,7 +3019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>4</v>
       </c>
@@ -2930,7 +3036,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>4</v>
       </c>
@@ -2947,7 +3053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>4</v>
       </c>
@@ -2964,7 +3070,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>4</v>
       </c>
@@ -2981,7 +3087,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>4</v>
       </c>
@@ -2998,7 +3104,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>4</v>
       </c>
@@ -3015,7 +3121,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>4</v>
       </c>
@@ -3032,7 +3138,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>4</v>
       </c>
@@ -3049,7 +3155,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>4</v>
       </c>
@@ -3066,7 +3172,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>4</v>
       </c>
@@ -3083,7 +3189,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>4</v>
       </c>
@@ -3100,7 +3206,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>4</v>
       </c>
@@ -3117,7 +3223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>4</v>
       </c>
@@ -3134,7 +3240,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>5</v>
       </c>
@@ -3151,7 +3257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>5</v>
       </c>
@@ -3168,7 +3274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>5</v>
       </c>
@@ -3185,7 +3291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>5</v>
       </c>
@@ -3202,7 +3308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>5</v>
       </c>
@@ -3219,7 +3325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>5</v>
       </c>
@@ -3236,7 +3342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>5</v>
       </c>
@@ -3253,7 +3359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>5</v>
       </c>
@@ -3270,7 +3376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>5</v>
       </c>
@@ -3287,7 +3393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>5</v>
       </c>
@@ -3304,7 +3410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>5</v>
       </c>
@@ -3321,7 +3427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>5</v>
       </c>
@@ -3338,7 +3444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>5</v>
       </c>
@@ -3355,7 +3461,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>5</v>
       </c>
@@ -3372,7 +3478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>5</v>
       </c>
@@ -3389,7 +3495,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>5</v>
       </c>
@@ -3406,7 +3512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>5</v>
       </c>
@@ -3423,7 +3529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>5</v>
       </c>
@@ -3440,7 +3546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>5</v>
       </c>
@@ -3457,7 +3563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>5</v>
       </c>
@@ -3474,7 +3580,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>5</v>
       </c>
@@ -3491,7 +3597,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>5</v>
       </c>
@@ -3508,7 +3614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>5</v>
       </c>
@@ -3525,7 +3631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>5</v>
       </c>
@@ -3542,7 +3648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>5</v>
       </c>
@@ -3559,7 +3665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>5</v>
       </c>
@@ -3576,7 +3682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>5</v>
       </c>
@@ -3593,7 +3699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>5</v>
       </c>
@@ -3610,7 +3716,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>5</v>
       </c>
@@ -3627,7 +3733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>5</v>
       </c>
@@ -3644,7 +3750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>5</v>
       </c>
@@ -3661,7 +3767,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>5</v>
       </c>
@@ -3678,7 +3784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>5</v>
       </c>
@@ -3695,7 +3801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>5</v>
       </c>
@@ -3712,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>5</v>
       </c>
@@ -3729,7 +3835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>5</v>
       </c>
@@ -3746,7 +3852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>5</v>
       </c>
@@ -3763,7 +3869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>5</v>
       </c>
@@ -3780,7 +3886,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>5</v>
       </c>
@@ -3797,7 +3903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>5</v>
       </c>
@@ -3814,7 +3920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>10</v>
       </c>
@@ -3831,7 +3937,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>10</v>
       </c>
@@ -3848,7 +3954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>10</v>
       </c>
@@ -3865,7 +3971,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>10</v>
       </c>
@@ -3882,7 +3988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>10</v>
       </c>
@@ -3899,7 +4005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>10</v>
       </c>
@@ -3916,7 +4022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>10</v>
       </c>
@@ -3933,7 +4039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>10</v>
       </c>
@@ -3950,7 +4056,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>10</v>
       </c>
@@ -3967,7 +4073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>10</v>
       </c>
@@ -3984,7 +4090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>10</v>
       </c>
@@ -4001,7 +4107,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>10</v>
       </c>
@@ -4018,7 +4124,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
         <v>10</v>
       </c>
@@ -4035,7 +4141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
         <v>10</v>
       </c>
@@ -4052,7 +4158,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
         <v>10</v>
       </c>
@@ -4069,7 +4175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
         <v>10</v>
       </c>
@@ -4086,7 +4192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
         <v>10</v>
       </c>
@@ -4103,7 +4209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
         <v>10</v>
       </c>
@@ -4120,7 +4226,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
         <v>10</v>
       </c>
@@ -4137,7 +4243,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
         <v>10</v>
       </c>
@@ -4154,7 +4260,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
         <v>10</v>
       </c>
@@ -4171,7 +4277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
         <v>10</v>
       </c>
@@ -4188,7 +4294,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
         <v>10</v>
       </c>
@@ -4205,7 +4311,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
         <v>10</v>
       </c>
@@ -4222,7 +4328,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
         <v>10</v>
       </c>
@@ -4239,7 +4345,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
         <v>10</v>
       </c>
@@ -4256,7 +4362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
         <v>10</v>
       </c>
@@ -4273,7 +4379,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
         <v>10</v>
       </c>
@@ -4290,7 +4396,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
         <v>10</v>
       </c>
@@ -4307,7 +4413,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
         <v>10</v>
       </c>
@@ -4324,7 +4430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
         <v>16</v>
       </c>
@@ -4341,7 +4447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
         <v>16</v>
       </c>
@@ -4358,7 +4464,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
         <v>16</v>
       </c>
@@ -4375,7 +4481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
         <v>16</v>
       </c>
@@ -4392,7 +4498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
         <v>16</v>
       </c>
@@ -4409,7 +4515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
         <v>16</v>
       </c>
@@ -4426,7 +4532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
         <v>16</v>
       </c>
@@ -4443,7 +4549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
         <v>16</v>
       </c>
@@ -4460,7 +4566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
         <v>16</v>
       </c>
@@ -4477,7 +4583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>16</v>
       </c>
@@ -4494,7 +4600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>16</v>
       </c>
@@ -4511,7 +4617,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
         <v>16</v>
       </c>
@@ -4528,7 +4634,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>16</v>
       </c>
@@ -4545,7 +4651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
         <v>16</v>
       </c>
@@ -4562,7 +4668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
         <v>16</v>
       </c>
@@ -4579,7 +4685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
         <v>16</v>
       </c>
@@ -4596,7 +4702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
         <v>16</v>
       </c>
@@ -4613,7 +4719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
         <v>16</v>
       </c>
@@ -4630,7 +4736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
         <v>16</v>
       </c>
@@ -4647,7 +4753,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
         <v>16</v>
       </c>
@@ -4664,7 +4770,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
         <v>16</v>
       </c>
@@ -4681,7 +4787,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
         <v>16</v>
       </c>
@@ -4698,7 +4804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
         <v>16</v>
       </c>
@@ -4715,7 +4821,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
         <v>16</v>
       </c>
@@ -4732,7 +4838,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
         <v>16</v>
       </c>
@@ -4749,7 +4855,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
         <v>16</v>
       </c>
@@ -4766,7 +4872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
         <v>16</v>
       </c>
@@ -4783,7 +4889,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
         <v>16</v>
       </c>
@@ -4800,7 +4906,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
         <v>16</v>
       </c>
@@ -4817,7 +4923,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
         <v>16</v>
       </c>

</xml_diff>